<commit_message>
"Learnings content added -> STL Tricks"
</commit_message>
<xml_diff>
--- a/My_CP_Track/CP.xlsx
+++ b/My_CP_Track/CP.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="293">
   <si>
     <t>Problem</t>
   </si>
@@ -1724,6 +1724,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">learnt to </t>
     </r>
     <r>
@@ -1739,6 +1746,30 @@
   </si>
   <si>
     <t>got corrective idea from Abhishek Saini sir</t>
+  </si>
+  <si>
+    <t>1973A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">had no ideas initially </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">learnt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>new framework to count pairs by taking part from set of elements</t>
+    </r>
+  </si>
+  <si>
+    <t>a new idea; but could have been though easily</t>
   </si>
   <si>
     <t>TOPIC</t>
@@ -3078,10 +3109,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -4238,6 +4269,26 @@
       </c>
       <c r="G61" s="13" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="62" ht="36" spans="1:7">
+      <c r="A62" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4269,7 +4320,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1">
         <v>1200</v>
@@ -4278,7 +4329,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="B3" s="2">
         <v>100000</v>
@@ -4286,7 +4337,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="B4" s="2">
         <v>100000</v>
@@ -4310,7 +4361,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="B7" s="2">
         <v>100000</v>
@@ -4318,7 +4369,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="B8" s="2">
         <v>100000</v>
@@ -4334,7 +4385,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="B10" s="3">
         <v>27</v>
@@ -4342,7 +4393,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="B11" s="3">
         <v>24</v>
@@ -4350,7 +4401,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="B12" s="3">
         <v>23</v>
@@ -4374,7 +4425,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="B15" s="3">
         <v>11</v>
@@ -4382,7 +4433,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="B16" s="3">
         <v>11</v>
@@ -4390,7 +4441,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B17" s="4">
         <v>8</v>
@@ -4398,7 +4449,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B18" s="4">
         <v>8</v>
@@ -4406,7 +4457,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="B19" s="4">
         <v>8</v>
@@ -4414,7 +4465,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B20" s="4">
         <v>4</v>
@@ -4422,7 +4473,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="4" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B21" s="4">
         <v>4</v>
@@ -4438,7 +4489,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -4446,7 +4497,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -4455,7 +4506,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -4463,7 +4514,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -4471,7 +4522,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="4" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
@@ -4479,7 +4530,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4487,7 +4538,7 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4495,7 +4546,7 @@
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4503,7 +4554,7 @@
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -4511,7 +4562,7 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4519,7 +4570,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4527,7 +4578,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4535,7 +4586,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -4543,7 +4594,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4551,7 +4602,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4559,7 +4610,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4587,7 +4638,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="B1" s="1">
         <v>1300</v>
@@ -4595,12 +4646,12 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:1">
@@ -4615,12 +4666,12 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -4630,17 +4681,17 @@
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:1">
@@ -4655,37 +4706,37 @@
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -4695,82 +4746,82 @@
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>